<commit_message>
Forgot the actual commit
</commit_message>
<xml_diff>
--- a/Recorded data/Clustering algorithms.xlsx
+++ b/Recorded data/Clustering algorithms.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fredrik-Oslo\Documents\Crowding_GA_with_SLS\Recorded data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D858C1-66A4-4A31-AA6C-7B058A210BF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA5447C-8EC8-415A-9F67-4969CD73AB8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1860" windowWidth="29040" windowHeight="18240" xr2:uid="{859EC958-069D-41C2-971F-BA92C576E400}"/>
+    <workbookView xWindow="-28920" yWindow="-1860" windowWidth="29040" windowHeight="18240" activeTab="1" xr2:uid="{859EC958-069D-41C2-971F-BA92C576E400}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="GA-innstillinger" sheetId="1" r:id="rId1"/>
+    <sheet name="Eksperiment 1 - Klyngingsalgori" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,20 +34,100 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>GA-innstillinger:</t>
   </si>
   <si>
     <t>25 runs per problem instance.</t>
+  </si>
+  <si>
+    <t>PopSize</t>
+  </si>
+  <si>
+    <t>Elitist niches</t>
+  </si>
+  <si>
+    <t>Tournament size</t>
+  </si>
+  <si>
+    <t>Pc</t>
+  </si>
+  <si>
+    <t>0.7</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>Pm</t>
+  </si>
+  <si>
+    <t>Init crowding</t>
+  </si>
+  <si>
+    <t>PID control rate</t>
+  </si>
+  <si>
+    <t>0.02</t>
+  </si>
+  <si>
+    <t>Wanted niches</t>
+  </si>
+  <si>
+    <t>Max members in niche</t>
+  </si>
+  <si>
+    <t>SLS-innstillinger:</t>
+  </si>
+  <si>
+    <t>Max-flips</t>
+  </si>
+  <si>
+    <t>Pn</t>
+  </si>
+  <si>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t>Max-flips in greedy SLS</t>
+  </si>
+  <si>
+    <t>Accepts first improvement</t>
+  </si>
+  <si>
+    <t>MaxFEs</t>
+  </si>
+  <si>
+    <t>DBScan</t>
+  </si>
+  <si>
+    <t>Bitflip-mutering I benchmark. Den andre for feature selection</t>
+  </si>
+  <si>
+    <t>Single point crossover</t>
+  </si>
+  <si>
+    <t>100k</t>
+  </si>
+  <si>
+    <t>Epsilon = 0.02</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -74,8 +155,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,25 +472,171 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A4D847-BB2F-4482-B2E5-BC5FA344E91B}">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15FAFA54-A2D7-40DF-AA16-09B830FBBF6D}">
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>1</v>
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Visualization now places dots logically in higher-dimensional problems.
</commit_message>
<xml_diff>
--- a/Recorded data/Clustering algorithms.xlsx
+++ b/Recorded data/Clustering algorithms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fredrik-Oslo\Documents\Crowding_GA_with_SLS\Recorded data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA5447C-8EC8-415A-9F67-4969CD73AB8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11869B8C-41D2-4086-A6AD-B436C1D069EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1860" windowWidth="29040" windowHeight="18240" activeTab="1" xr2:uid="{859EC958-069D-41C2-971F-BA92C576E400}"/>
+    <workbookView xWindow="-28920" yWindow="-1860" windowWidth="29040" windowHeight="18240" xr2:uid="{859EC958-069D-41C2-971F-BA92C576E400}"/>
   </bookViews>
   <sheets>
     <sheet name="GA-innstillinger" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>GA-innstillinger:</t>
   </si>
@@ -112,6 +112,33 @@
   </si>
   <si>
     <t>Epsilon = 0.02</t>
+  </si>
+  <si>
+    <t>Mapping bitstrings to numbers by parsing them as binary numbers, then normalizing to the search space.</t>
+  </si>
+  <si>
+    <t>Euclidean distance measure on the normalized axes.</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Dimensionality</t>
+  </si>
+  <si>
+    <t>Best</t>
+  </si>
+  <si>
+    <t>Worst</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>STD</t>
+  </si>
+  <si>
+    <t>Peak detection epsilon is 0.5*D</t>
   </si>
 </sst>
 </file>
@@ -472,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A4D847-BB2F-4482-B2E5-BC5FA344E91B}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,6 +637,21 @@
         <v>24</v>
       </c>
     </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -617,22 +659,60 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15FAFA54-A2D7-40DF-AA16-09B830FBBF6D}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A3:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>